<commit_message>
Finished data collection for basic probit 1997-2004
</commit_message>
<xml_diff>
--- a/data/failures/entities_start_end_dates.xlsx
+++ b/data/failures/entities_start_end_dates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9bf72e6496f26e8d/UWA PhD/bankFailure/data/failures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="11_BC803668C347457380E3C66D8CB5819721C9985F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F95408E-FE36-4EA4-84C2-A4AB5822B455}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="11_BC803668C347457380E3C66D8CB5819721C9985F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7A84A328-F372-41D8-A6E5-595FA3D1A967}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-11472" yWindow="1464" windowWidth="5328" windowHeight="3864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entsDates" sheetId="1" r:id="rId1"/>
-    <sheet name="code" sheetId="2" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId2"/>
+    <sheet name="code" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">entsDates!$A$1:$M$186</definedName>
@@ -38,8 +39,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={3AC5D5FA-6256-4BB4-BB45-3745274A3EBA}</author>
+    <author>emi</author>
     <author>tc={B8553458-24EB-4F46-AFDB-7DD7F84F49B4}</author>
-    <author>emi</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3AC5D5FA-6256-4BB4-BB45-3745274A3EBA}">
@@ -50,15 +51,7 @@
     This endDate is from entidades.dta database. It's approximante and is equal or lower than the true desappartiion date with a maximum of 3 months. Note that this is the date a bank disappears, it does not imply it failed but it could have been merged</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{B8553458-24EB-4F46-AFDB-7DD7F84F49B4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    fOR EXAMPLE, a financial company becomes a bank</t>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="2" shapeId="0" xr:uid="{11C43F25-94D5-46C7-8CF6-A0491A69A183}">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{DC00A26D-135E-4985-B64C-FF3091B0E578}">
       <text>
         <r>
           <rPr>
@@ -66,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>emi:</t>
         </r>
@@ -75,10 +68,349 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Include M&amp;A and volutary exit but not transformations</t>
+This is the date that any of the event for disappearing an entitiy occur</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{168B1AF7-FF2A-47E3-B5A8-A7F463051780}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Was this entity merged with another entitiy of similar size and a new entity emerged as a result?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{A7B2B9FB-BCFE-464E-8327-F5A6F4A8BAFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Was this disappearing entity adquired by a bigger entitiy and the aquiring entitiy preserved its name and status?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{6F58F602-4E18-4A39-90C4-5383259D8F28}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Any of ET_MERGE or ET_ADQUIRED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{44456A0B-B678-432B-B3CB-454447B6D959}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some assets were sold to another firm. A weaker form of ET_ADQUIRED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="2" shapeId="0" xr:uid="{B8553458-24EB-4F46-AFDB-7DD7F84F49B4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    fOR EXAMPLE, a financial company becomes a bank</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{F7BE579E-7247-42A8-8F0E-4129867C2334}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The entitiy ask the Central Bank to cancel its license. Article a) of Financial Entities Act</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{9ADCFC6A-9595-4CAA-9320-489F8C04E4F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Article d) in the Financial Entities Act</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0F9EB1A3-75C0-4C4B-9654-7E0F4C40877D}</author>
+    <author>emi</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{0F9EB1A3-75C0-4C4B-9654-7E0F4C40877D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This endDate is from entidades.dta database. It's approximante and is equal or lower than the true desappartiion date with a maximum of 3 months. Note that this is the date a bank disappears, it does not imply it failed but it could have been merged</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="1" shapeId="0" xr:uid="{BFE78514-93AF-4519-BE38-23264E1D83BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the date that any of the event for disappearing an entitiy occur</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="1" shapeId="0" xr:uid="{54607397-ACC6-4E7D-AB2C-D1E28485EEA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Was this entity merged with another entitiy of similar size and a new entity emerged as a result?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="1" shapeId="0" xr:uid="{3E70829C-CE17-457C-84CA-2344183B5B95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Was this disappearing entity adquired by a bigger entitiy and the aquiring entitiy preserved its name and status?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="1" shapeId="0" xr:uid="{AC1D7F39-CD84-4555-B3CB-A8E7AFA38653}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Any of ET_MERGE or ET_ADQUIRED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{97A6DFA9-2B28-42A3-B50E-B700C9DBDD12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Some assets were sold to another firm. A weaker form of ET_ADQUIRED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{8EFEA173-4C4D-49D7-8006-CA4469F9CF2D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The entitiy ask the Central Bank to cancel its license. Article a) of Financial Entities Act</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="1" shapeId="0" xr:uid="{7C55571B-5245-4DB8-888C-6F634C8AF4A9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>emi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Article d) in the Financial Entities Act</t>
         </r>
       </text>
     </comment>
@@ -87,7 +419,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="224">
   <si>
     <t>IDent</t>
   </si>
@@ -668,9 +1000,6 @@
     <t>entsDates</t>
   </si>
   <si>
-    <t>M_AND_A</t>
-  </si>
-  <si>
     <t>"transfiri'o activos y pasivos" It may hide a failure</t>
   </si>
   <si>
@@ -680,9 +1009,6 @@
     <t xml:space="preserve">Transfirió ALGUNOS activos y pasivos a Banco Río de la Plata S.A. y se revocó su autorización para funcionar.    </t>
   </si>
   <si>
-    <t>PARTIAL_SALE</t>
-  </si>
-  <si>
     <t>COMMENTS</t>
   </si>
   <si>
@@ -704,9 +1030,6 @@
     <t>ORDER_N</t>
   </si>
   <si>
-    <t>EXIT_DATE_XLS</t>
-  </si>
-  <si>
     <t>FIRST_DATE</t>
   </si>
   <si>
@@ -725,19 +1048,49 @@
     <t>Privatizado. Los privatizados son a solicitud del banco</t>
   </si>
   <si>
-    <t>Merge</t>
-  </si>
-  <si>
-    <t>Adquisition</t>
-  </si>
-  <si>
-    <t>TRANSFORMATION</t>
-  </si>
-  <si>
-    <t>VOLUNTARY_EXIT</t>
-  </si>
-  <si>
-    <t>FAIL_DATE_A</t>
+    <t>EXIT_DATE</t>
+  </si>
+  <si>
+    <t>ET_MERGE</t>
+  </si>
+  <si>
+    <t>ET_ADQUIRED</t>
+  </si>
+  <si>
+    <t>ET_OTHER</t>
+  </si>
+  <si>
+    <t>ET_PARTIAL_SALE</t>
+  </si>
+  <si>
+    <t>ET_TRANSFORMATION</t>
+  </si>
+  <si>
+    <t>ET_VOLUNTARY</t>
+  </si>
+  <si>
+    <t>Article d) in the Financial Entities Act</t>
+  </si>
+  <si>
+    <t>Exit Type Adquired: Was this disappearing entity adquired by a bigger entitiy and the aquiring entitiy preserved its name and status?</t>
+  </si>
+  <si>
+    <t>Exit Type Merge: Was this entity merged with another entitiy of similar size and a new entity emerged as a result?</t>
+  </si>
+  <si>
+    <t>Exit Type Merge or Adquisition: Any of ET_MERGE or ET_ADQUIRED</t>
+  </si>
+  <si>
+    <t>Exity Type Transfomration of institutional type: Change from bank to financial company, or state-owned bank to private bank</t>
+  </si>
+  <si>
+    <t>Exity Type Voluntary: The entitiy ask the Central Bank to cancel its license. Article a) of Financial Entities Act</t>
+  </si>
+  <si>
+    <t>Exity Type Partial Sale of some selected assets: Some assets were sold to another firm (Article c in the Financial Entities Act). A weaker form of ET_ADQUIRED. Corresponds to "Exclusión de activos y pasivos" and or "Se revocó su autorización para funcionar de acuerdo con lo previsto en el art. 44, inc. c),"</t>
+  </si>
+  <si>
+    <t>ET_MA</t>
   </si>
 </sst>
 </file>
@@ -759,14 +1112,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1128,56 +1481,63 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A4" dT="2021-02-17T02:06:03.95" personId="{20D3C5A8-94A4-4298-AF66-57B7A6F710B8}" id="{0F9EB1A3-75C0-4C4B-9654-7E0F4C40877D}">
+    <text>This endDate is from entidades.dta database. It's approximante and is equal or lower than the true desappartiion date with a maximum of 3 months. Note that this is the date a bank disappears, it does not imply it failed but it could have been merged</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" customWidth="1"/>
-    <col min="3" max="4" width="10.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.07421875" customWidth="1"/>
+    <col min="3" max="4" width="10.07421875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.61328125" customWidth="1"/>
+    <col min="6" max="6" width="6.69140625" customWidth="1"/>
+    <col min="7" max="7" width="10.23046875" customWidth="1"/>
+    <col min="9" max="9" width="9.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>214</v>
@@ -1186,13 +1546,13 @@
         <v>215</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1211,12 +1571,8 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="L2" s="2">
-        <f>E2*H2*K2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1232,15 +1588,11 @@
       <c r="E3" s="2">
         <v>38071</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <f t="shared" ref="L3:L18" si="0">E3*H3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1253,12 +1605,8 @@
       <c r="D4" s="1">
         <v>42248</v>
       </c>
-      <c r="L4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1277,12 +1625,8 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="L5" s="2">
-        <f t="shared" si="0"/>
-        <v>36769</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1295,12 +1639,8 @@
       <c r="D6" s="1">
         <v>43862</v>
       </c>
-      <c r="L6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1313,12 +1653,8 @@
       <c r="D7" s="1">
         <v>38412</v>
       </c>
-      <c r="L7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1331,12 +1667,8 @@
       <c r="D8" s="1">
         <v>43862</v>
       </c>
-      <c r="L8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1355,12 +1687,8 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="L9" s="2">
-        <f t="shared" si="0"/>
-        <v>35859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1373,12 +1701,8 @@
       <c r="D10" s="1">
         <v>43862</v>
       </c>
-      <c r="L10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1391,12 +1715,8 @@
       <c r="D11" s="1">
         <v>43862</v>
       </c>
-      <c r="L11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1409,12 +1729,8 @@
       <c r="D12" s="1">
         <v>43862</v>
       </c>
-      <c r="L12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1427,12 +1743,8 @@
       <c r="D13" s="1">
         <v>43862</v>
       </c>
-      <c r="L13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1451,15 +1763,11 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="M14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1472,12 +1780,8 @@
       <c r="D15" s="1">
         <v>43862</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1496,12 +1800,8 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="L16" s="2">
-        <f t="shared" si="0"/>
-        <v>36097</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1514,12 +1814,8 @@
       <c r="D17" s="1">
         <v>43862</v>
       </c>
-      <c r="L17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1532,12 +1828,8 @@
       <c r="D18" s="1">
         <v>43862</v>
       </c>
-      <c r="L18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1551,7 +1843,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1571,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1585,7 +1877,7 @@
         <v>37226</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1601,8 +1893,11 @@
       <c r="E22" s="2">
         <v>37363</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1616,7 +1911,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1925,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1650,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1676,10 +1971,10 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1699,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1735,8 +2030,11 @@
       <c r="E29" s="2">
         <v>35684</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1752,8 +2050,11 @@
       <c r="E30" s="2">
         <v>37397</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1767,7 +2068,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1787,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1803,8 +2104,11 @@
       <c r="E33" s="2">
         <v>36223</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1818,7 +2122,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1841,10 +2145,10 @@
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1864,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1887,10 +2191,10 @@
         <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1904,7 +2208,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1927,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1941,7 +2245,7 @@
         <v>40422</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1964,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1978,7 +2282,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1992,7 +2296,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2008,11 +2312,14 @@
       <c r="E44" s="2">
         <v>36867</v>
       </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
       <c r="M44" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2026,7 +2333,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2040,7 +2347,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2054,7 +2361,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2077,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2093,8 +2400,11 @@
       <c r="E49" s="2">
         <v>37426</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2110,8 +2420,11 @@
       <c r="E50" s="2">
         <v>35558</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2134,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2148,7 +2461,7 @@
         <v>38596</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2168,10 +2481,10 @@
         <v>1</v>
       </c>
       <c r="M53" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2185,7 +2498,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2199,7 +2512,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2215,8 +2528,11 @@
       <c r="E56" s="2">
         <v>37727</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2232,8 +2548,11 @@
       <c r="E57" s="2">
         <v>36188</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2247,7 +2566,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2263,8 +2582,11 @@
       <c r="E59" s="2">
         <v>37357</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2287,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2303,8 +2625,11 @@
       <c r="E61" s="2">
         <v>35481</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2320,8 +2645,11 @@
       <c r="E62" s="2">
         <v>36081</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2335,7 +2663,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2355,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2378,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2394,8 +2722,11 @@
       <c r="E66" s="2">
         <v>37137</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2411,8 +2742,11 @@
       <c r="E67" s="2">
         <v>36126</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2426,7 +2760,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2440,7 +2774,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2456,8 +2790,14 @@
       <c r="E70" s="2">
         <v>36465</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2480,10 +2820,10 @@
         <v>1</v>
       </c>
       <c r="M71" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2503,10 +2843,10 @@
         <v>1</v>
       </c>
       <c r="M72" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2520,7 +2860,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2536,8 +2876,11 @@
       <c r="E74" s="2">
         <v>35880</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2557,10 +2900,10 @@
         <v>1</v>
       </c>
       <c r="M75" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2574,7 +2917,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2590,8 +2933,11 @@
       <c r="E77" s="2">
         <v>37395</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2611,10 +2957,10 @@
         <v>1</v>
       </c>
       <c r="M78" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2628,7 +2974,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2644,8 +2990,11 @@
       <c r="E80" s="2">
         <v>37004</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2659,7 +3008,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2673,7 +3022,7 @@
         <v>39052</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2687,7 +3036,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2707,10 +3056,10 @@
         <v>1</v>
       </c>
       <c r="M84" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2724,7 +3073,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2738,7 +3087,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2754,8 +3103,11 @@
       <c r="E87" s="2">
         <v>37434</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2778,10 +3130,10 @@
         <v>1</v>
       </c>
       <c r="M88" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2801,10 +3153,10 @@
         <v>1</v>
       </c>
       <c r="M89" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2818,7 +3170,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2838,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2852,7 +3204,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2866,7 +3218,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2882,8 +3234,11 @@
       <c r="E94" s="2">
         <v>35971</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2897,7 +3252,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2911,7 +3266,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2925,7 +3280,7 @@
         <v>42156</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2939,7 +3294,7 @@
         <v>39234</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2953,7 +3308,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2967,7 +3322,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2981,7 +3336,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2995,7 +3350,7 @@
         <v>43070</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -3009,7 +3364,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -3023,7 +3378,7 @@
         <v>41609</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -3039,8 +3394,11 @@
       <c r="E105" s="2">
         <v>35859</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -3060,7 +3418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -3074,7 +3432,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -3088,7 +3446,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -3102,7 +3460,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -3116,7 +3474,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -3132,8 +3490,11 @@
       <c r="E111" s="2">
         <v>35776</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -3149,8 +3510,11 @@
       <c r="E112" s="2">
         <v>37395</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -3164,7 +3528,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -3181,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -3201,7 +3565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -3221,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -3235,7 +3599,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -3258,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -3272,7 +3636,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -3286,7 +3650,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -3309,10 +3673,10 @@
         <v>1</v>
       </c>
       <c r="M121" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -3332,7 +3696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -3346,7 +3710,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -3362,8 +3726,11 @@
       <c r="E124" s="2">
         <v>36896</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -3383,10 +3750,10 @@
         <v>1</v>
       </c>
       <c r="M125" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -3402,8 +3769,11 @@
       <c r="E126" s="2">
         <v>36266</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -3423,10 +3793,10 @@
         <v>1</v>
       </c>
       <c r="M127" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -3440,7 +3810,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -3454,7 +3824,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -3468,7 +3838,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -3482,7 +3852,7 @@
         <v>40238</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -3496,7 +3866,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -3516,10 +3886,10 @@
         <v>1</v>
       </c>
       <c r="M133" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -3533,7 +3903,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -3547,7 +3917,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -3561,7 +3931,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -3575,7 +3945,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -3589,7 +3959,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -3603,7 +3973,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -3617,7 +3987,7 @@
         <v>39326</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -3631,7 +4001,7 @@
         <v>39965</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -3645,7 +4015,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -3659,7 +4029,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -3673,7 +4043,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -3687,7 +4057,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -3701,7 +4071,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -3715,7 +4085,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -3729,7 +4099,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -3743,7 +4113,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -3759,8 +4129,11 @@
       <c r="E150" s="2">
         <v>35922</v>
       </c>
-    </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="K150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -3776,8 +4149,11 @@
       <c r="E151" s="2">
         <v>38030</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -3797,10 +4173,10 @@
         <v>1</v>
       </c>
       <c r="M152" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -3820,10 +4196,10 @@
         <v>1</v>
       </c>
       <c r="M153" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3837,7 +4213,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3851,7 +4227,7 @@
         <v>42430</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -3865,7 +4241,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -3885,10 +4261,10 @@
         <v>1</v>
       </c>
       <c r="M157" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -3908,10 +4284,10 @@
         <v>1</v>
       </c>
       <c r="M158" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -3925,7 +4301,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -3945,7 +4321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -3959,7 +4335,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -3973,7 +4349,7 @@
         <v>40148</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -3987,7 +4363,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -4001,7 +4377,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -4015,7 +4391,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -4029,7 +4405,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -4043,7 +4419,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -4063,7 +4439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -4077,7 +4453,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -4091,7 +4467,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -4105,7 +4481,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -4121,8 +4497,11 @@
       <c r="E172" s="2">
         <v>36672</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -4136,7 +4515,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -4150,7 +4529,7 @@
         <v>39417</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -4164,7 +4543,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -4184,7 +4563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -4198,7 +4577,7 @@
         <v>38412</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -4214,8 +4593,11 @@
       <c r="E178" s="2">
         <v>37011</v>
       </c>
-    </row>
-    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -4235,10 +4617,10 @@
         <v>1</v>
       </c>
       <c r="M179" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -4252,7 +4634,7 @@
         <v>41518</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -4275,10 +4657,10 @@
         <v>1</v>
       </c>
       <c r="M181" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -4298,7 +4680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -4314,8 +4696,11 @@
       <c r="E183" s="2">
         <v>37210</v>
       </c>
-    </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -4335,10 +4720,10 @@
         <v>1</v>
       </c>
       <c r="M184" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -4352,7 +4737,7 @@
         <v>43862</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -4368,14 +4753,12 @@
       <c r="E186" s="2">
         <v>35901</v>
       </c>
+      <c r="I186">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M186" xr:uid="{F766B230-6C83-4273-BA2E-06188A6384CC}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="312"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M186">
       <sortCondition ref="B1:B186"/>
     </sortState>
@@ -4387,6 +4770,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E00769-3751-4D15-B1B7-797B88611919}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="31.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D4D6D3-7FE6-4C80-A8FC-BC1BB47FAC69}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -4394,39 +4882,39 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>192</v>
       </c>

</xml_diff>